<commit_message>
Loppuraportti ja Jaakon arviointilomake valmis
</commit_message>
<xml_diff>
--- a/Muu/evaluationForm.xlsx
+++ b/Muu/evaluationForm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheikkil\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J4sK4\Desktop\Koodailut\ohjelmistokehityksen-sovellusprojekti-2k19\Muu\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC105BA0-265E-460B-B396-C51E0781AE4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="11430"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="toveriarvio" sheetId="1" r:id="rId1"/>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,7 +542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -651,15 +652,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x01010075A879D650EAF1439071501626B9B673" ma:contentTypeVersion="0" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="cae2cb75c228908d568ecf0dda734541">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efa2e1335bef07a6688a5da4ccafe8a1">
     <xsd:element name="properties">
@@ -773,6 +765,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -780,14 +781,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFA0A5C4-2B1B-41DE-8A26-A2E577BE6887}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0437064-5E6F-49DF-A3BD-914D3F13A663}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -799,6 +792,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFA0A5C4-2B1B-41DE-8A26-A2E577BE6887}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>